<commit_message>
Add animation to category toggle
</commit_message>
<xml_diff>
--- a/Risk Analysis Tool.xlsx
+++ b/Risk Analysis Tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Thantry\Documents\Assignments\IS301\Assignment 1\Risk Analysis Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A442E5C-7D3B-48B5-A6D6-881FBEBCF18F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D9049A-5094-45B4-9707-11F63B841192}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E72CB985-5F28-407E-912B-397E368FB384}"/>
   </bookViews>
@@ -566,11 +566,68 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -581,6 +638,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -590,15 +653,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,60 +660,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -979,7 +979,7 @@
   <dimension ref="B1:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="48" zoomScaleNormal="48" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -991,965 +991,965 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:14" ht="36.5" thickTop="1" x14ac:dyDescent="0.8">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="2:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="18"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="37"/>
       <c r="N3" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="31"/>
       <c r="N4" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="31"/>
       <c r="N5" s="1">
         <f t="shared" ref="N5:N10" si="0">IF(ISNUMBER(SEARCH("Yes",M5)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="24"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="31"/>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="24"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="31"/>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="24"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="31"/>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="24"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="31"/>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="24"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="27"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="7" t="str">
         <f>SUM(N4:N10) &amp; "/28"</f>
         <v>0/28</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="18"/>
+      <c r="B13" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="37"/>
       <c r="N13" s="9"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="24"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
       <c r="N14" s="10">
         <f>IF(ISNUMBER(SEARCH("Yes",M14)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="24"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="31"/>
       <c r="N15" s="10">
         <f>IF(ISNUMBER(SEARCH("Yes",M15)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="24"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
       <c r="N16" s="11">
         <f>IF(ISNUMBER(SEARCH("Yes",M16)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="31"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="35"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="24"/>
       <c r="N17" s="8" t="str">
         <f>SUM(N14:N16) &amp; "/9"</f>
         <v>0/9</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="18"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="37"/>
       <c r="N19" s="9"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="24"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="31"/>
       <c r="N20" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M20)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="24"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="31"/>
       <c r="N21" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M21)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="24"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="31"/>
       <c r="N22" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M22)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="24"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="31"/>
       <c r="N23" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M23)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="24"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="31"/>
       <c r="N24" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M24)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="31"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="35"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="24"/>
       <c r="N25" s="6" t="str">
         <f>SUM(N20:N24) &amp; "/16"</f>
         <v>0/16</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B26" s="38"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="18"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="37"/>
       <c r="N27" s="12"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="24"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="31"/>
       <c r="N28" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M28)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="24"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="31"/>
       <c r="N29" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M29)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="24"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="31"/>
       <c r="N30" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M30)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="30"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="34"/>
       <c r="N31" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M31)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="40"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="41"/>
-      <c r="M32" s="42"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="16"/>
       <c r="N32" s="2" t="str">
         <f>SUM(N28:N31) &amp; "/13"</f>
         <v>0/13</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B33" s="31"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="34"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="18"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="37"/>
       <c r="N34" s="9"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="24"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="31"/>
       <c r="N35" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M35)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="24"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
+      <c r="M36" s="31"/>
       <c r="N36" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M36)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="30"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="34"/>
       <c r="N37" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M37)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="40"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41"/>
-      <c r="M38" s="42"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="16"/>
       <c r="N38" s="2" t="str">
         <f>SUM(N35:N37) &amp; "/10"</f>
         <v>0/10</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B39" s="31"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
       <c r="N39" s="3"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="18"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="37"/>
       <c r="N40" s="9"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="24"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="31"/>
       <c r="N41" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M41)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="24"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
+      <c r="L42" s="30"/>
+      <c r="M42" s="31"/>
       <c r="N42" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M42)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="24"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="30"/>
+      <c r="L43" s="30"/>
+      <c r="M43" s="31"/>
       <c r="N43" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M43)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="30"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="34"/>
       <c r="N44" s="4">
         <f>IF(ISNUMBER(SEARCH("Yes",M44)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="40"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="41"/>
-      <c r="L45" s="41"/>
-      <c r="M45" s="42"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="16"/>
       <c r="N45" s="2" t="str">
         <f>SUM(N41:N44) &amp; "/13"</f>
         <v>0/13</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B46" s="31"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="34"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
       <c r="N46" s="3"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
-      <c r="M47" s="18"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="36"/>
+      <c r="M47" s="37"/>
       <c r="N47" s="9"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="23"/>
-      <c r="M48" s="24"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
+      <c r="L48" s="30"/>
+      <c r="M48" s="31"/>
       <c r="N48" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="23"/>
-      <c r="M49" s="24"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="30"/>
+      <c r="K49" s="30"/>
+      <c r="L49" s="30"/>
+      <c r="M49" s="31"/>
       <c r="N49" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="30"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="33"/>
+      <c r="L50" s="33"/>
+      <c r="M50" s="34"/>
       <c r="N50" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="40"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="41"/>
-      <c r="K51" s="41"/>
-      <c r="L51" s="41"/>
-      <c r="M51" s="42"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="16"/>
       <c r="N51" s="2" t="str">
         <f>SUM(N48:N50) &amp; "/11"</f>
         <v>0/11</v>
       </c>
     </row>
     <row r="52" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="32"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="33"/>
-      <c r="J52" s="33"/>
-      <c r="K52" s="33"/>
-      <c r="L52" s="33"/>
-      <c r="M52" s="33"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
       <c r="N52" s="1"/>
     </row>
     <row r="53" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="43"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="45"/>
-      <c r="K53" s="14" t="s">
+      <c r="B53" s="19"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
+      <c r="L53" s="39"/>
+      <c r="M53" s="39"/>
       <c r="N53" s="5" t="str">
         <f>SUM(N4:N10,N14:N16,N20:N24,N28:N31,N35:N37,N41:N44,N48:N50) &amp; "/100"</f>
         <v>0/100</v>
@@ -1958,21 +1958,37 @@
     <row r="54" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B51:M51"/>
-    <mergeCell ref="B52:M52"/>
-    <mergeCell ref="B53:J53"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B38:M38"/>
-    <mergeCell ref="B39:M39"/>
-    <mergeCell ref="B45:M45"/>
-    <mergeCell ref="B46:M46"/>
+    <mergeCell ref="B21:M21"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:M10"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B31:M31"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="B36:M36"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="B24:M24"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="B30:M30"/>
     <mergeCell ref="B17:M17"/>
     <mergeCell ref="B12:M12"/>
     <mergeCell ref="B18:M18"/>
     <mergeCell ref="B25:M25"/>
     <mergeCell ref="B48:M48"/>
-    <mergeCell ref="B49:M49"/>
-    <mergeCell ref="B50:M50"/>
     <mergeCell ref="B40:M40"/>
     <mergeCell ref="B41:M41"/>
     <mergeCell ref="B42:M42"/>
@@ -1984,33 +2000,17 @@
     <mergeCell ref="B37:M37"/>
     <mergeCell ref="B22:M22"/>
     <mergeCell ref="B23:M23"/>
-    <mergeCell ref="B24:M24"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B28:M28"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="B30:M30"/>
-    <mergeCell ref="B31:M31"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="B36:M36"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="B51:M51"/>
+    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B38:M38"/>
+    <mergeCell ref="B39:M39"/>
+    <mergeCell ref="B45:M45"/>
+    <mergeCell ref="B46:M46"/>
+    <mergeCell ref="B49:M49"/>
+    <mergeCell ref="B50:M50"/>
     <mergeCell ref="K53:M53"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B21:M21"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:M10"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B16:M16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add all categories to categories div and add appropriate JS
</commit_message>
<xml_diff>
--- a/Risk Analysis Tool.xlsx
+++ b/Risk Analysis Tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Thantry\Documents\Assignments\IS301\Assignment 1\Risk Analysis Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D9049A-5094-45B4-9707-11F63B841192}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86B6C98-EA5A-48AD-A469-0268903AD487}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E72CB985-5F28-407E-912B-397E368FB384}"/>
   </bookViews>
@@ -566,51 +566,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -620,6 +575,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -629,37 +611,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -978,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AF9427-E6C0-4DE0-9D2D-B5611002D649}">
   <dimension ref="B1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="48" zoomScaleNormal="48" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="48" zoomScaleNormal="48" workbookViewId="0">
+      <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -991,965 +991,965 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:14" ht="36.5" thickTop="1" x14ac:dyDescent="0.8">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="25"/>
     </row>
     <row r="3" spans="2:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="37"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="22"/>
       <c r="N3" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="31"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="16"/>
       <c r="N4" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="31"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="16"/>
       <c r="N5" s="1">
         <f t="shared" ref="N5:N10" si="0">IF(ISNUMBER(SEARCH("Yes",M5)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="31"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="16"/>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="31"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="16"/>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="31"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="31"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="16"/>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="31"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="16"/>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="45"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="19"/>
       <c r="N11" s="7" t="str">
         <f>SUM(N4:N10) &amp; "/28"</f>
         <v>0/28</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="37"/>
+      <c r="B13" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="22"/>
       <c r="N13" s="9"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="31"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="16"/>
       <c r="N14" s="10">
         <f>IF(ISNUMBER(SEARCH("Yes",M14)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="31"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="16"/>
       <c r="N15" s="10">
         <f>IF(ISNUMBER(SEARCH("Yes",M15)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="31"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="16"/>
       <c r="N16" s="11">
         <f>IF(ISNUMBER(SEARCH("Yes",M16)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="24"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="36"/>
       <c r="N17" s="8" t="str">
         <f>SUM(N14:N16) &amp; "/9"</f>
         <v>0/9</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="22"/>
       <c r="N19" s="9"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="31"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="16"/>
       <c r="N20" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M20)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="31"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="16"/>
       <c r="N21" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M21)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="31"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="16"/>
       <c r="N22" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M22)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="31"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="16"/>
       <c r="N23" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M23)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="31"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="16"/>
       <c r="N24" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M24)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="22"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="24"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="36"/>
       <c r="N25" s="6" t="str">
         <f>SUM(N20:N24) &amp; "/16"</f>
         <v>0/16</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="37"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="22"/>
       <c r="N27" s="12"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="31"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="16"/>
       <c r="N28" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M28)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="31"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="16"/>
       <c r="N29" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M29)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="31"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="16"/>
       <c r="N30" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M30)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="34"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="28"/>
       <c r="N31" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M31)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="16"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="33"/>
       <c r="N32" s="2" t="str">
         <f>SUM(N28:N31) &amp; "/13"</f>
         <v>0/13</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="37"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="22"/>
       <c r="N34" s="9"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="31"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="16"/>
       <c r="N35" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M35)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="31"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="16"/>
       <c r="N36" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M36)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="34"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="28"/>
       <c r="N37" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M37)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="14"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="16"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
+      <c r="M38" s="33"/>
       <c r="N38" s="2" t="str">
         <f>SUM(N35:N37) &amp; "/10"</f>
         <v>0/10</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B39" s="22"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="35"/>
       <c r="N39" s="3"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="37"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="22"/>
       <c r="N40" s="9"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
-      <c r="L41" s="30"/>
-      <c r="M41" s="31"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="16"/>
       <c r="N41" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M41)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="31"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="16"/>
       <c r="N42" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M42)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="30"/>
-      <c r="L43" s="30"/>
-      <c r="M43" s="31"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="16"/>
       <c r="N43" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M43)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="33"/>
-      <c r="L44" s="33"/>
-      <c r="M44" s="34"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="28"/>
       <c r="N44" s="4">
         <f>IF(ISNUMBER(SEARCH("Yes",M44)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="14"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="16"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="33"/>
       <c r="N45" s="2" t="str">
         <f>SUM(N41:N44) &amp; "/13"</f>
         <v>0/13</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B46" s="22"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="23"/>
-      <c r="M46" s="23"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
       <c r="N46" s="3"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="37"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="22"/>
       <c r="N47" s="9"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="31"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="16"/>
       <c r="N48" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="30"/>
-      <c r="M49" s="31"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="16"/>
       <c r="N49" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="32" t="s">
+      <c r="B50" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="33"/>
-      <c r="L50" s="33"/>
-      <c r="M50" s="34"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="28"/>
       <c r="N50" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="14"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
-      <c r="M51" s="16"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
+      <c r="L51" s="32"/>
+      <c r="M51" s="33"/>
       <c r="N51" s="2" t="str">
         <f>SUM(N48:N50) &amp; "/11"</f>
         <v>0/11</v>
       </c>
     </row>
     <row r="52" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
-      <c r="M52" s="18"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="40"/>
+      <c r="J52" s="40"/>
+      <c r="K52" s="40"/>
+      <c r="L52" s="40"/>
+      <c r="M52" s="40"/>
       <c r="N52" s="1"/>
     </row>
     <row r="53" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="19"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="21"/>
-      <c r="K53" s="38" t="s">
+      <c r="B53" s="41"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
+      <c r="H53" s="42"/>
+      <c r="I53" s="42"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="L53" s="39"/>
-      <c r="M53" s="39"/>
+      <c r="L53" s="45"/>
+      <c r="M53" s="45"/>
       <c r="N53" s="5" t="str">
         <f>SUM(N4:N10,N14:N16,N20:N24,N28:N31,N35:N37,N41:N44,N48:N50) &amp; "/100"</f>
         <v>0/100</v>
@@ -1958,50 +1958,6 @@
     <row r="54" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B21:M21"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:M10"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B16:M16"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B31:M31"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="B36:M36"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="B32:M32"/>
-    <mergeCell ref="B24:M24"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B28:M28"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="B30:M30"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="B12:M12"/>
-    <mergeCell ref="B18:M18"/>
-    <mergeCell ref="B25:M25"/>
-    <mergeCell ref="B48:M48"/>
-    <mergeCell ref="B40:M40"/>
-    <mergeCell ref="B41:M41"/>
-    <mergeCell ref="B42:M42"/>
-    <mergeCell ref="B43:M43"/>
-    <mergeCell ref="B44:M44"/>
-    <mergeCell ref="B47:M47"/>
-    <mergeCell ref="B19:M19"/>
-    <mergeCell ref="B20:M20"/>
-    <mergeCell ref="B37:M37"/>
-    <mergeCell ref="B22:M22"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="B51:M51"/>
-    <mergeCell ref="B52:M52"/>
     <mergeCell ref="B53:J53"/>
     <mergeCell ref="B33:M33"/>
     <mergeCell ref="B38:M38"/>
@@ -2011,6 +1967,50 @@
     <mergeCell ref="B49:M49"/>
     <mergeCell ref="B50:M50"/>
     <mergeCell ref="K53:M53"/>
+    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="B22:M22"/>
+    <mergeCell ref="B23:M23"/>
+    <mergeCell ref="B51:M51"/>
+    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="B48:M48"/>
+    <mergeCell ref="B40:M40"/>
+    <mergeCell ref="B41:M41"/>
+    <mergeCell ref="B42:M42"/>
+    <mergeCell ref="B43:M43"/>
+    <mergeCell ref="B44:M44"/>
+    <mergeCell ref="B47:M47"/>
+    <mergeCell ref="B24:M24"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B29:M29"/>
+    <mergeCell ref="B30:M30"/>
+    <mergeCell ref="B25:M25"/>
+    <mergeCell ref="B31:M31"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="B36:M36"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="B21:M21"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:M10"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="B19:M19"/>
+    <mergeCell ref="B20:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add font awesome and change the assessment criteria
</commit_message>
<xml_diff>
--- a/Risk Analysis Tool.xlsx
+++ b/Risk Analysis Tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Thantry\Documents\Assignments\IS301\Assignment 1\Risk Analysis Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86B6C98-EA5A-48AD-A469-0268903AD487}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85827EB4-EAB2-4DB6-A8A6-B36D69EFD920}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E72CB985-5F28-407E-912B-397E368FB384}"/>
   </bookViews>
@@ -566,6 +566,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -575,13 +599,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -593,6 +629,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,64 +647,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -978,7 +978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AF9427-E6C0-4DE0-9D2D-B5611002D649}">
   <dimension ref="B1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="48" zoomScaleNormal="48" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
@@ -991,965 +991,965 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:14" ht="36.5" thickTop="1" x14ac:dyDescent="0.8">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="25"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="40"/>
     </row>
     <row r="3" spans="2:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="22"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="34"/>
       <c r="N3" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="16"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="24"/>
       <c r="N4" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="16"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
       <c r="N5" s="1">
         <f t="shared" ref="N5:N10" si="0">IF(ISNUMBER(SEARCH("Yes",M5)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="16"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="24"/>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="16"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="24"/>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="24"/>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="16"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="24"/>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="16"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="24"/>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="19"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="7" t="str">
         <f>SUM(N4:N10) &amp; "/28"</f>
         <v>0/28</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="22"/>
+      <c r="B13" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="34"/>
       <c r="N13" s="9"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="16"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="24"/>
       <c r="N14" s="10">
         <f>IF(ISNUMBER(SEARCH("Yes",M14)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="16"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="24"/>
       <c r="N15" s="10">
         <f>IF(ISNUMBER(SEARCH("Yes",M15)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="16"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="24"/>
       <c r="N16" s="11">
         <f>IF(ISNUMBER(SEARCH("Yes",M16)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="36"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="35"/>
       <c r="N17" s="8" t="str">
         <f>SUM(N14:N16) &amp; "/9"</f>
         <v>0/9</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="22"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="34"/>
       <c r="N19" s="9"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="16"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="24"/>
       <c r="N20" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M20)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="16"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="24"/>
       <c r="N21" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M21)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="16"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="24"/>
       <c r="N22" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M22)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="16"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="24"/>
       <c r="N23" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M23)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="16"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="24"/>
       <c r="N24" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M24)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="36"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="35"/>
       <c r="N25" s="6" t="str">
         <f>SUM(N20:N24) &amp; "/16"</f>
         <v>0/16</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="22"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="34"/>
       <c r="N27" s="12"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="16"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="24"/>
       <c r="N28" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M28)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="16"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="24"/>
       <c r="N29" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M29)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="16"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="24"/>
       <c r="N30" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M30)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="28"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="27"/>
       <c r="N31" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M31)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="31"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="33"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="21"/>
       <c r="N32" s="2" t="str">
         <f>SUM(N28:N31) &amp; "/13"</f>
         <v>0/13</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="22"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="34"/>
       <c r="N34" s="9"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="16"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="24"/>
       <c r="N35" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M35)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="16"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="24"/>
       <c r="N36" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M36)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="28"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="27"/>
       <c r="N37" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M37)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="31"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="33"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="21"/>
       <c r="N38" s="2" t="str">
         <f>SUM(N35:N37) &amp; "/10"</f>
         <v>0/10</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B39" s="34"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="35"/>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
       <c r="N39" s="3"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="22"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="34"/>
       <c r="N40" s="9"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="16"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="24"/>
       <c r="N41" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M41)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="16"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="24"/>
       <c r="N42" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M42)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="16"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="24"/>
       <c r="N43" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M43)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="28"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="27"/>
       <c r="N44" s="4">
         <f>IF(ISNUMBER(SEARCH("Yes",M44)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="31"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="33"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="21"/>
       <c r="N45" s="2" t="str">
         <f>SUM(N41:N44) &amp; "/13"</f>
         <v>0/13</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B46" s="34"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="35"/>
-      <c r="K46" s="35"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="35"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
       <c r="N46" s="3"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="21"/>
-      <c r="M47" s="22"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="33"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="34"/>
       <c r="N47" s="9"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="16"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="24"/>
       <c r="N48" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="16"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="24"/>
       <c r="N49" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="27"/>
-      <c r="L50" s="27"/>
-      <c r="M50" s="28"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="27"/>
       <c r="N50" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="31"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="33"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="21"/>
       <c r="N51" s="2" t="str">
         <f>SUM(N48:N50) &amp; "/11"</f>
         <v>0/11</v>
       </c>
     </row>
     <row r="52" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="39"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="40"/>
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="40"/>
-      <c r="J52" s="40"/>
-      <c r="K52" s="40"/>
-      <c r="L52" s="40"/>
-      <c r="M52" s="40"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="31"/>
+      <c r="K52" s="31"/>
+      <c r="L52" s="31"/>
+      <c r="M52" s="31"/>
       <c r="N52" s="1"/>
     </row>
     <row r="53" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="41"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="42"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="44" t="s">
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L53" s="45"/>
-      <c r="M53" s="45"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="29"/>
       <c r="N53" s="5" t="str">
         <f>SUM(N4:N10,N14:N16,N20:N24,N28:N31,N35:N37,N41:N44,N48:N50) &amp; "/100"</f>
         <v>0/100</v>
@@ -1958,16 +1958,33 @@
     <row r="54" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B53:J53"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B38:M38"/>
-    <mergeCell ref="B39:M39"/>
-    <mergeCell ref="B45:M45"/>
-    <mergeCell ref="B46:M46"/>
-    <mergeCell ref="B49:M49"/>
-    <mergeCell ref="B50:M50"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="B21:M21"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:M10"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="B19:M19"/>
+    <mergeCell ref="B20:M20"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="B25:M25"/>
+    <mergeCell ref="B31:M31"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="B36:M36"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B32:M32"/>
     <mergeCell ref="B22:M22"/>
     <mergeCell ref="B23:M23"/>
     <mergeCell ref="B51:M51"/>
@@ -1984,33 +2001,16 @@
     <mergeCell ref="B28:M28"/>
     <mergeCell ref="B29:M29"/>
     <mergeCell ref="B30:M30"/>
-    <mergeCell ref="B25:M25"/>
-    <mergeCell ref="B31:M31"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="B36:M36"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="B32:M32"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B12:M12"/>
-    <mergeCell ref="B21:M21"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:M10"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B16:M16"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="B18:M18"/>
-    <mergeCell ref="B19:M19"/>
-    <mergeCell ref="B20:M20"/>
+    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B38:M38"/>
+    <mergeCell ref="B39:M39"/>
+    <mergeCell ref="B45:M45"/>
+    <mergeCell ref="B46:M46"/>
+    <mergeCell ref="B49:M49"/>
+    <mergeCell ref="B50:M50"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="B37:M37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Make risk 2 3 and 4 use riskIssues() function
</commit_message>
<xml_diff>
--- a/Risk Analysis Tool.xlsx
+++ b/Risk Analysis Tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurav Thantry\Documents\Assignments\IS301\Assignment 1\Risk Analysis Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85827EB4-EAB2-4DB6-A8A6-B36D69EFD920}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FC98CC-227A-4C78-ACB6-6F2627222358}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E72CB985-5F28-407E-912B-397E368FB384}"/>
   </bookViews>
@@ -566,30 +566,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -599,6 +575,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -608,58 +632,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -991,965 +991,965 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:14" ht="36.5" thickTop="1" x14ac:dyDescent="0.8">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="40"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="2:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="34"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="27"/>
       <c r="N3" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="16"/>
       <c r="N4" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="16"/>
       <c r="N5" s="1">
         <f t="shared" ref="N5:N10" si="0">IF(ISNUMBER(SEARCH("Yes",M5)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="24"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="16"/>
       <c r="N6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="24"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="16"/>
       <c r="N7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="24"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
       <c r="N8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="24"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="16"/>
       <c r="N9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="24"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="16"/>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="45"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="19"/>
       <c r="N11" s="7" t="str">
         <f>SUM(N4:N10) &amp; "/28"</f>
         <v>0/28</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="34"/>
+      <c r="B13" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
       <c r="N13" s="9"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="24"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="16"/>
       <c r="N14" s="10">
         <f>IF(ISNUMBER(SEARCH("Yes",M14)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="24"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="16"/>
       <c r="N15" s="10">
         <f>IF(ISNUMBER(SEARCH("Yes",M15)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="24"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="16"/>
       <c r="N16" s="11">
         <f>IF(ISNUMBER(SEARCH("Yes",M16)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="35"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="22"/>
       <c r="N17" s="8" t="str">
         <f>SUM(N14:N16) &amp; "/9"</f>
         <v>0/9</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="34"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
       <c r="N19" s="9"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="24"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="16"/>
       <c r="N20" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M20)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="24"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="16"/>
       <c r="N21" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M21)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="24"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="16"/>
       <c r="N22" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M22)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="24"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="16"/>
       <c r="N23" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M23)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="24"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="16"/>
       <c r="N24" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M24)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="35"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="22"/>
       <c r="N25" s="6" t="str">
         <f>SUM(N20:N24) &amp; "/16"</f>
         <v>0/16</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="37"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="34"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="27"/>
       <c r="N27" s="12"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="24"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="16"/>
       <c r="N28" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M28)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="24"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="16"/>
       <c r="N29" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M29)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="24"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="16"/>
       <c r="N30" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M30)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="27"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="35"/>
       <c r="N31" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M31)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="21"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="38"/>
       <c r="N32" s="2" t="str">
         <f>SUM(N28:N31) &amp; "/13"</f>
         <v>0/13</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="34"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="27"/>
       <c r="N34" s="9"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="24"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="16"/>
       <c r="N35" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M35)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="24"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="16"/>
       <c r="N36" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M36)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="27"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
+      <c r="K37" s="34"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="35"/>
       <c r="N37" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M37)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="21"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="37"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="38"/>
       <c r="N38" s="2" t="str">
         <f>SUM(N35:N37) &amp; "/10"</f>
         <v>0/10</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B39" s="17"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
       <c r="N39" s="3"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
-      <c r="M40" s="34"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="27"/>
       <c r="N40" s="9"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="23"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="23"/>
-      <c r="M41" s="24"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="16"/>
       <c r="N41" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M41)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="24"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="16"/>
       <c r="N42" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M42)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="24"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="16"/>
       <c r="N43" s="1">
         <f>IF(ISNUMBER(SEARCH("Yes",M43)),3,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="26"/>
-      <c r="M44" s="27"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="34"/>
+      <c r="M44" s="35"/>
       <c r="N44" s="4">
         <f>IF(ISNUMBER(SEARCH("Yes",M44)),4,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="21"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="38"/>
       <c r="N45" s="2" t="str">
         <f>SUM(N41:N44) &amp; "/13"</f>
         <v>0/13</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B46" s="17"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
       <c r="N46" s="3"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="34"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="27"/>
       <c r="N47" s="9"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="23"/>
-      <c r="M48" s="24"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="16"/>
       <c r="N48" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="23"/>
-      <c r="M49" s="24"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="16"/>
       <c r="N49" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="25" t="s">
+      <c r="B50" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="27"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="34"/>
+      <c r="L50" s="34"/>
+      <c r="M50" s="35"/>
       <c r="N50" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="21"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="38"/>
       <c r="N51" s="2" t="str">
         <f>SUM(N48:N50) &amp; "/11"</f>
         <v>0/11</v>
       </c>
     </row>
     <row r="52" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="30"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="31"/>
-      <c r="I52" s="31"/>
-      <c r="J52" s="31"/>
-      <c r="K52" s="31"/>
-      <c r="L52" s="31"/>
-      <c r="M52" s="31"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="40"/>
+      <c r="J52" s="40"/>
+      <c r="K52" s="40"/>
+      <c r="L52" s="40"/>
+      <c r="M52" s="40"/>
       <c r="N52" s="1"/>
     </row>
     <row r="53" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="14"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="16"/>
-      <c r="K53" s="28" t="s">
+      <c r="B53" s="41"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
+      <c r="H53" s="42"/>
+      <c r="I53" s="42"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="L53" s="29"/>
-      <c r="M53" s="29"/>
+      <c r="L53" s="45"/>
+      <c r="M53" s="45"/>
       <c r="N53" s="5" t="str">
         <f>SUM(N4:N10,N14:N16,N20:N24,N28:N31,N35:N37,N41:N44,N48:N50) &amp; "/100"</f>
         <v>0/100</v>
@@ -1958,33 +1958,16 @@
     <row r="54" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B21:M21"/>
-    <mergeCell ref="B8:M8"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:M10"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="B16:M16"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="B18:M18"/>
-    <mergeCell ref="B19:M19"/>
-    <mergeCell ref="B20:M20"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B12:M12"/>
-    <mergeCell ref="B25:M25"/>
-    <mergeCell ref="B31:M31"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B35:M35"/>
-    <mergeCell ref="B36:M36"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B38:M38"/>
+    <mergeCell ref="B39:M39"/>
+    <mergeCell ref="B45:M45"/>
+    <mergeCell ref="B46:M46"/>
+    <mergeCell ref="B49:M49"/>
+    <mergeCell ref="B50:M50"/>
+    <mergeCell ref="K53:M53"/>
+    <mergeCell ref="B37:M37"/>
     <mergeCell ref="B22:M22"/>
     <mergeCell ref="B23:M23"/>
     <mergeCell ref="B51:M51"/>
@@ -2001,16 +1984,33 @@
     <mergeCell ref="B28:M28"/>
     <mergeCell ref="B29:M29"/>
     <mergeCell ref="B30:M30"/>
-    <mergeCell ref="B53:J53"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B38:M38"/>
-    <mergeCell ref="B39:M39"/>
-    <mergeCell ref="B45:M45"/>
-    <mergeCell ref="B46:M46"/>
-    <mergeCell ref="B49:M49"/>
-    <mergeCell ref="B50:M50"/>
-    <mergeCell ref="K53:M53"/>
-    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="B25:M25"/>
+    <mergeCell ref="B31:M31"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B35:M35"/>
+    <mergeCell ref="B36:M36"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B32:M32"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="B21:M21"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:M10"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="B19:M19"/>
+    <mergeCell ref="B20:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>